<commit_message>
Bugs fixed, added .bat file
</commit_message>
<xml_diff>
--- a/example/mp3_app/xls/E_MP3_0.xlsx
+++ b/example/mp3_app/xls/E_MP3_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Karolina\watson-assistant-workbench\example\mp3_app\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{989E0958-ED29-4C0E-8186-AA92BFD4DC6C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{475A02A1-7512-4888-A170-BA1EC907624F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11670" xr2:uid="{355F90E0-CA55-4E54-A039-E09B9EABB366}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>Názvy mp3 se pak ukládají spolu s činností do textového souboru.</t>
   </si>
   <si>
-    <t>//V případě, že je více možných reakcí, se názvy uloží za sebe.</t>
-  </si>
-  <si>
-    <t>//Názvy mp3 souborů jsou pojmenované čísleně ve formátu 00X.</t>
+    <t>V případě, že je více možných reakcí, se názvy uloží za sebe.</t>
+  </si>
+  <si>
+    <t>Názvy mp3 souborů jsou pojmenované čísleně ve formátu 00X.</t>
   </si>
 </sst>
 </file>

</xml_diff>